<commit_message>
edit coverage file location
</commit_message>
<xml_diff>
--- a/trachoma/data/coverage/scen2a.xlsx
+++ b/trachoma/data/coverage/scen2a.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewgraham/Dropbox/TrachomaGitHub/ntd-model-trachoma/trachoma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewgraham/Dropbox/ntd-model-trachoma/trachoma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A781C008-0B7A-8D4D-8F53-F971EF0A9938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CC509B-3862-1D4B-91A2-A25B007AB1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12380" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{4BA44B84-CD41-6346-982B-221FCFDB0FEF}"/>
   </bookViews>
@@ -428,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1646A6-EB47-2E4C-B241-E23BF391ECB5}">
-  <dimension ref="A1:BZ3"/>
+  <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,196 +483,103 @@
         <v>2024.0833333333333</v>
       </c>
       <c r="P1">
-        <v>2024.5</v>
+        <v>2025</v>
       </c>
       <c r="Q1">
-        <v>2024.5833333333333</v>
+        <v>2025.0833333333333</v>
       </c>
       <c r="R1">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="S1">
-        <v>2025.0833333333333</v>
+        <v>2026.0833333333333</v>
       </c>
       <c r="T1">
-        <v>2025.5</v>
+        <v>2027</v>
       </c>
       <c r="U1">
-        <v>2025.5833333333333</v>
+        <v>2027.0833333333333</v>
       </c>
       <c r="V1">
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="W1">
-        <v>2026.0833333333333</v>
+        <v>2028.0833333333333</v>
       </c>
       <c r="X1">
-        <v>2026.5</v>
+        <v>2029</v>
       </c>
       <c r="Y1">
-        <v>2026.5833333333333</v>
+        <v>2029.0833333333333</v>
       </c>
       <c r="Z1">
-        <v>2027</v>
+        <v>2030</v>
       </c>
       <c r="AA1">
-        <v>2027.0833333333333</v>
+        <v>2030.0833333333333</v>
       </c>
       <c r="AB1">
-        <v>2027.5</v>
+        <v>2031</v>
       </c>
       <c r="AC1">
-        <v>2027.5833333333333</v>
+        <v>2031.0833333333333</v>
       </c>
       <c r="AD1">
-        <v>2028</v>
+        <v>2032</v>
       </c>
       <c r="AE1">
-        <v>2028.0833333333333</v>
+        <v>2032.0833333333333</v>
       </c>
       <c r="AF1">
-        <v>2028.5</v>
+        <v>2033</v>
       </c>
       <c r="AG1">
-        <v>2028.5833333333333</v>
+        <v>2033.0833333333333</v>
       </c>
       <c r="AH1">
-        <v>2029</v>
+        <v>2034</v>
       </c>
       <c r="AI1">
-        <v>2029.0833333333333</v>
+        <v>2034.0833333333333</v>
       </c>
       <c r="AJ1">
-        <v>2029.5</v>
+        <v>2035</v>
       </c>
       <c r="AK1">
-        <v>2029.5833333333333</v>
+        <v>2035.0833333333333</v>
       </c>
       <c r="AL1">
-        <v>2030</v>
+        <v>2036</v>
       </c>
       <c r="AM1">
-        <v>2030.0833333333333</v>
+        <v>2036.0833333333333</v>
       </c>
       <c r="AN1">
-        <v>2030.5</v>
+        <v>2037</v>
       </c>
       <c r="AO1">
-        <v>2030.5833333333333</v>
+        <v>2037.0833333333333</v>
       </c>
       <c r="AP1">
-        <v>2031</v>
+        <v>2038</v>
       </c>
       <c r="AQ1">
-        <v>2031.0833333333333</v>
+        <v>2038.0833333333333</v>
       </c>
       <c r="AR1">
-        <v>2031.5</v>
+        <v>2039</v>
       </c>
       <c r="AS1">
-        <v>2031.5833333333333</v>
+        <v>2039.0833333333333</v>
       </c>
       <c r="AT1">
-        <v>2032</v>
+        <v>2040</v>
       </c>
       <c r="AU1">
-        <v>2032.0833333333333</v>
-      </c>
-      <c r="AV1">
-        <v>2032.5</v>
-      </c>
-      <c r="AW1">
-        <v>2032.5833333333333</v>
-      </c>
-      <c r="AX1">
-        <v>2033</v>
-      </c>
-      <c r="AY1">
-        <v>2033.0833333333333</v>
-      </c>
-      <c r="AZ1">
-        <v>2033.5</v>
-      </c>
-      <c r="BA1">
-        <v>2033.5833333333333</v>
-      </c>
-      <c r="BB1">
-        <v>2034</v>
-      </c>
-      <c r="BC1">
-        <v>2034.0833333333333</v>
-      </c>
-      <c r="BD1">
-        <v>2034.5</v>
-      </c>
-      <c r="BE1">
-        <v>2034.5833333333333</v>
-      </c>
-      <c r="BF1">
-        <v>2035</v>
-      </c>
-      <c r="BG1">
-        <v>2035.0833333333333</v>
-      </c>
-      <c r="BH1">
-        <v>2035.5</v>
-      </c>
-      <c r="BI1">
-        <v>2035.5833333333333</v>
-      </c>
-      <c r="BJ1">
-        <v>2036</v>
-      </c>
-      <c r="BK1">
-        <v>2036.0833333333333</v>
-      </c>
-      <c r="BL1">
-        <v>2036.5</v>
-      </c>
-      <c r="BM1">
-        <v>2036.5833333333333</v>
-      </c>
-      <c r="BN1">
-        <v>2037</v>
-      </c>
-      <c r="BO1">
-        <v>2037.0833333333333</v>
-      </c>
-      <c r="BP1">
-        <v>2037.5</v>
-      </c>
-      <c r="BQ1">
-        <v>2037.5833333333333</v>
-      </c>
-      <c r="BR1">
-        <v>2038</v>
-      </c>
-      <c r="BS1">
-        <v>2038.0833333333333</v>
-      </c>
-      <c r="BT1">
-        <v>2038.5</v>
-      </c>
-      <c r="BU1">
-        <v>2038.5833333333333</v>
-      </c>
-      <c r="BV1">
-        <v>2039</v>
-      </c>
-      <c r="BW1">
-        <v>2039.0833333333333</v>
-      </c>
-      <c r="BX1">
-        <v>2039.5</v>
-      </c>
-      <c r="BY1">
-        <v>2039.5833333333333</v>
-      </c>
-      <c r="BZ1">
-        <v>2040</v>
+        <v>2040.0833333333301</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -760,56 +667,8 @@
       <c r="AT2">
         <v>0.85</v>
       </c>
-      <c r="AV2">
-        <v>0.85</v>
-      </c>
-      <c r="AX2">
-        <v>0.85</v>
-      </c>
-      <c r="AZ2">
-        <v>0.85</v>
-      </c>
-      <c r="BB2">
-        <v>0.85</v>
-      </c>
-      <c r="BD2">
-        <v>0.85</v>
-      </c>
-      <c r="BF2">
-        <v>0.85</v>
-      </c>
-      <c r="BH2">
-        <v>0.85</v>
-      </c>
-      <c r="BJ2">
-        <v>0.85</v>
-      </c>
-      <c r="BL2">
-        <v>0.85</v>
-      </c>
-      <c r="BN2">
-        <v>0.85</v>
-      </c>
-      <c r="BP2">
-        <v>0.85</v>
-      </c>
-      <c r="BR2">
-        <v>0.85</v>
-      </c>
-      <c r="BT2">
-        <v>0.85</v>
-      </c>
-      <c r="BV2">
-        <v>0.85</v>
-      </c>
-      <c r="BX2">
-        <v>0.85</v>
-      </c>
-      <c r="BZ2">
-        <v>0.85</v>
-      </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -877,51 +736,6 @@
         <v>0.85</v>
       </c>
       <c r="AU3">
-        <v>0.85</v>
-      </c>
-      <c r="AW3">
-        <v>0.85</v>
-      </c>
-      <c r="AY3">
-        <v>0.85</v>
-      </c>
-      <c r="BA3">
-        <v>0.85</v>
-      </c>
-      <c r="BC3">
-        <v>0.85</v>
-      </c>
-      <c r="BE3">
-        <v>0.85</v>
-      </c>
-      <c r="BG3">
-        <v>0.85</v>
-      </c>
-      <c r="BI3">
-        <v>0.85</v>
-      </c>
-      <c r="BK3">
-        <v>0.85</v>
-      </c>
-      <c r="BM3">
-        <v>0.85</v>
-      </c>
-      <c r="BO3">
-        <v>0.85</v>
-      </c>
-      <c r="BQ3">
-        <v>0.85</v>
-      </c>
-      <c r="BS3">
-        <v>0.85</v>
-      </c>
-      <c r="BU3">
-        <v>0.85</v>
-      </c>
-      <c r="BW3">
-        <v>0.85</v>
-      </c>
-      <c r="BY3">
         <v>0.85</v>
       </c>
     </row>

</xml_diff>